<commit_message>
Fix error calculation in RC.py and update outputs
Corrected the denominator in the error calculation for sy and sy_probe from sqrt(6) to sqrt(3) for more accurate uncertainty estimation. Added print statements for debugging. Updated RC_exp_fit.png and logbook_parte1modifica.xlsx to reflect new results.
</commit_message>
<xml_diff>
--- a/Physics_lab/RC-Oamp_introduction/logbook_parte1modifica.xlsx
+++ b/Physics_lab/RC-Oamp_introduction/logbook_parte1modifica.xlsx
@@ -2058,11 +2058,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="430739"/>
-        <c:axId val="95535349"/>
+        <c:axId val="74283215"/>
+        <c:axId val="85672350"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="430739"/>
+        <c:axId val="74283215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2130,12 +2130,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="95535349"/>
+        <c:crossAx val="85672350"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="95535349"/>
+        <c:axId val="85672350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,7 +2203,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="430739"/>
+        <c:crossAx val="74283215"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2303,10 +2303,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14372209187921"/>
-          <c:y val="0.167289952630267"/>
-          <c:w val="0.753273291455385"/>
-          <c:h val="0.661181750186986"/>
+          <c:x val="0.143732970027248"/>
+          <c:y val="0.167310809126044"/>
+          <c:w val="0.753178928247048"/>
+          <c:h val="0.661139508789428"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2393,11 +2393,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="98719692"/>
-        <c:axId val="56793636"/>
+        <c:axId val="30291762"/>
+        <c:axId val="15045437"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98719692"/>
+        <c:axId val="30291762"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2476,12 +2476,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="56793636"/>
+        <c:crossAx val="15045437"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56793636"/>
+        <c:axId val="15045437"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2529,8 +2529,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0470748505259971"/>
-              <c:y val="0.426950885066068"/>
+              <c:x val="0.0470784135634272"/>
+              <c:y val="0.426754768732078"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2568,7 +2568,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98719692"/>
+        <c:crossAx val="30291762"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2669,10 +2669,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.143627116070751"/>
-          <c:y val="0.167150979153506"/>
-          <c:w val="0.753359143703029"/>
-          <c:h val="0.661276058117498"/>
+          <c:x val="0.143638020042514"/>
+          <c:y val="0.167172100075815"/>
+          <c:w val="0.753264500455512"/>
+          <c:h val="0.661233257518322"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2759,11 +2759,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="40967340"/>
-        <c:axId val="9912956"/>
+        <c:axId val="56466480"/>
+        <c:axId val="41820957"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40967340"/>
+        <c:axId val="56466480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2842,12 +2842,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9912956"/>
+        <c:crossAx val="41820957"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="9912956"/>
+        <c:axId val="41820957"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2895,8 +2895,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.046990055416382"/>
-              <c:y val="0.427037271004422"/>
+              <c:x val="0.0469936228363195"/>
+              <c:y val="0.426838514025777"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2934,7 +2934,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40967340"/>
+        <c:crossAx val="56466480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3184,11 +3184,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="34601672"/>
-        <c:axId val="33197444"/>
+        <c:axId val="82555235"/>
+        <c:axId val="38017663"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="34601672"/>
+        <c:axId val="82555235"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3256,12 +3256,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33197444"/>
+        <c:crossAx val="38017663"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="33197444"/>
+        <c:axId val="38017663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3329,7 +3329,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34601672"/>
+        <c:crossAx val="82555235"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3582,11 +3582,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="64199642"/>
-        <c:axId val="88332113"/>
+        <c:axId val="90672130"/>
+        <c:axId val="44375319"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64199642"/>
+        <c:axId val="90672130"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3666,12 +3666,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="88332113"/>
+        <c:crossAx val="44375319"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="88332113"/>
+        <c:axId val="44375319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3748,7 +3748,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="64199642"/>
+        <c:crossAx val="90672130"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3997,11 +3997,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="18108881"/>
-        <c:axId val="4270063"/>
+        <c:axId val="99758999"/>
+        <c:axId val="73792261"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="18108881"/>
+        <c:axId val="99758999"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4069,12 +4069,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4270063"/>
+        <c:crossAx val="73792261"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="4270063"/>
+        <c:axId val="73792261"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4142,7 +4142,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18108881"/>
+        <c:crossAx val="99758999"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4391,11 +4391,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="19565765"/>
-        <c:axId val="21405135"/>
+        <c:axId val="59791486"/>
+        <c:axId val="51200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="19565765"/>
+        <c:axId val="59791486"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4463,12 +4463,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21405135"/>
+        <c:crossAx val="51200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="21405135"/>
+        <c:axId val="51200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4536,7 +4536,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19565765"/>
+        <c:crossAx val="59791486"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4636,10 +4636,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.143773902897517"/>
-          <c:y val="0.167085164260306"/>
-          <c:w val="0.753419329746548"/>
-          <c:h val="0.661226197949362"/>
+          <c:x val="0.143783223129781"/>
+          <c:y val="0.167102647274249"/>
+          <c:w val="0.75333851938286"/>
+          <c:h val="0.661190750235429"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -4726,11 +4726,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="46454794"/>
-        <c:axId val="8254176"/>
+        <c:axId val="11495989"/>
+        <c:axId val="4976460"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="46454794"/>
+        <c:axId val="11495989"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4809,12 +4809,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8254176"/>
+        <c:crossAx val="4976460"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="8254176"/>
+        <c:axId val="4976460"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4862,8 +4862,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.0469955273222273"/>
-              <c:y val="0.427286043105252"/>
+              <c:x val="0.0469985738363801"/>
+              <c:y val="0.427121481636497"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -4901,7 +4901,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46454794"/>
+        <c:crossAx val="11495989"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5002,10 +5002,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.156671375369205"/>
-          <c:y val="0.167170401250651"/>
-          <c:w val="0.710414793887248"/>
-          <c:h val="0.64960917144346"/>
+          <c:x val="0.156681435818404"/>
+          <c:y val="0.167187825724411"/>
+          <c:w val="0.71039619854877"/>
+          <c:h val="0.64957264957265"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5092,11 +5092,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1746063"/>
-        <c:axId val="32410147"/>
+        <c:axId val="33424454"/>
+        <c:axId val="63807556"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1746063"/>
+        <c:axId val="33424454"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5188,12 +5188,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32410147"/>
+        <c:crossAx val="63807556"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32410147"/>
+        <c:axId val="63807556"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5272,7 +5272,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1746063"/>
+        <c:crossAx val="33424454"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5373,10 +5373,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.156666273723918"/>
-          <c:y val="0.167095979392989"/>
-          <c:w val="0.710538724507839"/>
-          <c:h val="0.649680815320865"/>
+          <c:x val="0.156675508399646"/>
+          <c:y val="0.167114695340502"/>
+          <c:w val="0.7105216622458"/>
+          <c:h val="0.649641577060932"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5463,11 +5463,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="12306467"/>
-        <c:axId val="36888245"/>
+        <c:axId val="1747769"/>
+        <c:axId val="51646269"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12306467"/>
+        <c:axId val="1747769"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5559,12 +5559,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36888245"/>
+        <c:crossAx val="51646269"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36888245"/>
+        <c:axId val="51646269"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5643,7 +5643,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12306467"/>
+        <c:crossAx val="1747769"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5744,10 +5744,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.143681214421252"/>
-          <c:y val="0.167289952630267"/>
-          <c:w val="0.753320683111954"/>
-          <c:h val="0.661181750186986"/>
+          <c:x val="0.143692120844087"/>
+          <c:y val="0.167310809126044"/>
+          <c:w val="0.753226051313193"/>
+          <c:h val="0.661139508789428"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -5834,11 +5834,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="62126786"/>
-        <c:axId val="62622172"/>
+        <c:axId val="53521429"/>
+        <c:axId val="83319689"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="62126786"/>
+        <c:axId val="53521429"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5917,12 +5917,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62622172"/>
+        <c:crossAx val="83319689"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="62622172"/>
+        <c:axId val="83319689"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5970,8 +5970,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.047134724857685"/>
-              <c:y val="0.426950885066068"/>
+              <c:x val="0.0471383027174738"/>
+              <c:y val="0.426754768732078"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -6009,7 +6009,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62126786"/>
+        <c:crossAx val="53521429"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6073,9 +6073,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>753840</xdr:colOff>
+      <xdr:colOff>753480</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>430560</xdr:rowOff>
+      <xdr:rowOff>430200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6083,8 +6083,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15512040" y="2118600"/>
-        <a:ext cx="5798520" cy="3303000"/>
+        <a:off x="15526080" y="2118600"/>
+        <a:ext cx="5806800" cy="3302640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6103,9 +6103,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>742680</xdr:colOff>
+      <xdr:colOff>742320</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>427320</xdr:rowOff>
+      <xdr:rowOff>426960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6113,8 +6113,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="22053960" y="2115360"/>
-        <a:ext cx="5798520" cy="3303000"/>
+        <a:off x="22078080" y="2115360"/>
+        <a:ext cx="5807160" cy="3302640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6133,9 +6133,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>253080</xdr:colOff>
+      <xdr:colOff>252720</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6143,8 +6143,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7867440" y="12426480"/>
-        <a:ext cx="7208280" cy="3975480"/>
+        <a:off x="7869960" y="12426480"/>
+        <a:ext cx="7219440" cy="3975120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6163,9 +6163,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>750960</xdr:colOff>
+      <xdr:colOff>750600</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6173,8 +6173,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15509160" y="5938920"/>
-        <a:ext cx="5798520" cy="3296880"/>
+        <a:off x="15523200" y="5938920"/>
+        <a:ext cx="5806800" cy="3296520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6193,9 +6193,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>743040</xdr:colOff>
+      <xdr:colOff>742680</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6203,8 +6203,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="22054320" y="5959800"/>
-        <a:ext cx="5798520" cy="3296880"/>
+        <a:off x="22078440" y="5959800"/>
+        <a:ext cx="5807160" cy="3296520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6223,9 +6223,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>785520</xdr:colOff>
+      <xdr:colOff>785160</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6238,8 +6238,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15557040" y="9514440"/>
-          <a:ext cx="5785200" cy="3351240"/>
+          <a:off x="15571080" y="9514440"/>
+          <a:ext cx="5793480" cy="3350880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6260,9 +6260,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>745920</xdr:colOff>
+      <xdr:colOff>745560</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>110880</xdr:rowOff>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6275,45 +6275,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22082400" y="9501480"/>
-          <a:ext cx="5773320" cy="3344040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="0">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>284040</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>322920</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Immagine 3" descr=""/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip r:embed="rId8"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8570520" y="2131560"/>
-          <a:ext cx="6575040" cy="6554880"/>
+          <a:off x="22106520" y="9501480"/>
+          <a:ext cx="5781960" cy="3343680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6334,13 +6297,50 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>475200</xdr:colOff>
+      <xdr:colOff>474840</xdr:colOff>
       <xdr:row>92</xdr:row>
-      <xdr:rowOff>84240</xdr:rowOff>
+      <xdr:rowOff>83880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Immagine 4" descr=""/>
+        <xdr:cNvPr id="7" name="Immagine 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId8"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295200" y="12423960"/>
+          <a:ext cx="6811920" cy="3957120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>653760</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>222480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>259200</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Immagine 3" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -6349,8 +6349,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="295200" y="12423960"/>
-          <a:ext cx="6811200" cy="3957480"/>
+          <a:off x="8926920" y="2070000"/>
+          <a:ext cx="6168960" cy="6168960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6376,9 +6376,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>473400</xdr:colOff>
+      <xdr:colOff>473040</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>68760</xdr:rowOff>
+      <xdr:rowOff>68400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6387,7 +6387,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5757480" y="4724280"/>
-        <a:ext cx="5553360" cy="3440520"/>
+        <a:ext cx="5553000" cy="3440160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6406,9 +6406,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>314640</xdr:colOff>
+      <xdr:colOff>314280</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6417,7 +6417,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5545800" y="10212480"/>
-        <a:ext cx="5606280" cy="3453840"/>
+        <a:ext cx="5605920" cy="3453480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6436,9 +6436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>397440</xdr:colOff>
+      <xdr:colOff>397080</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6452,7 +6452,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7992360" y="816120"/>
-          <a:ext cx="6465600" cy="3755520"/>
+          <a:ext cx="6465240" cy="3755160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6473,9 +6473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>559080</xdr:colOff>
+      <xdr:colOff>558720</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:rowOff>5400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6485,7 +6485,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14636160" y="804960"/>
-          <a:ext cx="6429960" cy="3734640"/>
+          <a:ext cx="6429600" cy="3734280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6543,9 +6543,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>447120</xdr:colOff>
+      <xdr:colOff>446760</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>118440</xdr:rowOff>
+      <xdr:rowOff>118080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6554,7 +6554,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5824080" y="3672000"/>
-        <a:ext cx="6107400" cy="3214080"/>
+        <a:ext cx="6107040" cy="3213720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6578,9 +6578,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>399240</xdr:colOff>
+      <xdr:colOff>398880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6589,7 +6589,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="805680" y="5667120"/>
-        <a:ext cx="4742640" cy="2887560"/>
+        <a:ext cx="4742280" cy="2887200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6608,9 +6608,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>727200</xdr:colOff>
+      <xdr:colOff>726840</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6619,7 +6619,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="6257880" y="5667120"/>
-        <a:ext cx="4756320" cy="2887560"/>
+        <a:ext cx="4755960" cy="2887200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6638,9 +6638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>410040</xdr:colOff>
+      <xdr:colOff>409680</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>134640</xdr:rowOff>
+      <xdr:rowOff>134280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -6649,7 +6649,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="5149080" y="10248840"/>
-        <a:ext cx="4741920" cy="2849040"/>
+        <a:ext cx="4741560" cy="2848680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -6670,11 +6670,11 @@
   </sheetPr>
   <dimension ref="B1:O1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A106" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J103" activeCellId="0" sqref="J103"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
@@ -7191,7 +7191,7 @@
         <v>38</v>
       </c>
       <c r="C37" s="12" t="n">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="D37" s="48" t="n">
         <v>12</v>
@@ -7676,7 +7676,7 @@
       <selection pane="topLeft" activeCell="P42" activeCellId="0" sqref="P42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.86"/>
@@ -12131,7 +12131,7 @@
       <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.14"/>
@@ -12385,7 +12385,7 @@
       <selection pane="topLeft" activeCell="B76" activeCellId="0" sqref="B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.88"/>

</xml_diff>